<commit_message>
Commit von Excel funktion welche eine neue Excel Datei erstellt und die Zeilen von der Exceldatei in eine Mitarbeiter Liste Verarbeitet
</commit_message>
<xml_diff>
--- a/src/main/resources/Excel/Wichtige_Dinge_Dienstplan.xlsx
+++ b/src/main/resources/Excel/Wichtige_Dinge_Dienstplan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\paulr\IdeaProjects\SYP\DienstplanWebapp\src\main\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9948D4-70BF-4D0E-811F-0C05C87898DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC58CFA-F597-4AD5-A769-A3763DEF593F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1428" yWindow="1428" windowWidth="17280" windowHeight="8964" xr2:uid="{2F10E949-AEAE-4B7C-AAC8-72FF2755CB85}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{2F10E949-AEAE-4B7C-AAC8-72FF2755CB85}"/>
   </bookViews>
   <sheets>
     <sheet name="Ausgangsdatei" sheetId="2" r:id="rId1"/>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AEEB860-A6BA-470A-AEA9-D49D966C4D54}">
   <dimension ref="A1:AH16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="AH16" sqref="AH16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V12" sqref="V12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>